<commit_message>
update cancer_vaccine.tsv about disease column(all completed)
</commit_message>
<xml_diff>
--- a/src/templates/cancer_vaccine_MONDO.xlsx
+++ b/src/templates/cancer_vaccine_MONDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AE67D2-3F30-0C4A-B5D0-70D3BB4D2320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CDD849-D025-334B-8092-8317E101C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="680" windowWidth="28240" windowHeight="17040" xr2:uid="{922C2959-0093-1E49-9E88-C387A27C2EFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>http://purl.obolibrary.org/obo/MONDO_0007254</t>
   </si>
@@ -197,6 +197,10 @@
   </si>
   <si>
     <t>lymphoma</t>
+  </si>
+  <si>
+    <t>disease</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -594,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F39B9E-8F82-5546-9B39-8E8CB52CC082}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -788,6 +792,11 @@
       </c>
       <c r="B23" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed immunizes disease column, and update MONDO.xlsx
</commit_message>
<xml_diff>
--- a/src/templates/cancer_vaccine_MONDO.xlsx
+++ b/src/templates/cancer_vaccine_MONDO.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CDD849-D025-334B-8092-8317E101C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB1E559-F253-5C42-80EF-0AF9D101A36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="680" windowWidth="28240" windowHeight="17040" xr2:uid="{922C2959-0093-1E49-9E88-C387A27C2EFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>http://purl.obolibrary.org/obo/MONDO_0007254</t>
   </si>
@@ -106,16 +106,7 @@
     <t>renal cancer </t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/MONDO_0005089</t>
-  </si>
-  <si>
     <t>sarcoma</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/MONDO_0007576</t>
-  </si>
-  <si>
-    <t>esophageal cancer </t>
   </si>
   <si>
     <t>head and neck cancer</t>
@@ -175,10 +166,6 @@
     <t>http://purl.obolibrary.org/obo/MONDO_0005233</t>
   </si>
   <si>
-    <t>non-small cell lung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>prostate cancer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -199,7 +186,171 @@
     <t>lymphoma</t>
   </si>
   <si>
-    <t>disease</t>
+    <t>cancer name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MONDO or DOID link</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bile duct cancer</t>
+  </si>
+  <si>
+    <t>comments</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0003059</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>melanoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DOID_1909</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cholangiocarcinoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0019087</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>osteosarcoma</t>
+  </si>
+  <si>
+    <t>esophageal cancer</t>
+  </si>
+  <si>
+    <t>gastric adenocarcinoma</t>
+  </si>
+  <si>
+    <t>Ewing sarcoma</t>
+  </si>
+  <si>
+    <t>glioblastoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GVHD</t>
+  </si>
+  <si>
+    <t>head and neck squamous cell carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0007576</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005036</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0012817</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0018177</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0013730</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0009807</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0010150</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hematologic disorder</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005570</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPV associated cancer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lip and oral cavity carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0023644</t>
+  </si>
+  <si>
+    <t>oropharyngeal carcinoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0044926</t>
+  </si>
+  <si>
+    <t>rectal cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0006519</t>
+  </si>
+  <si>
+    <t>small intestine cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0000956</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005089</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mantle cell lymphoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0018876</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0008433</t>
+  </si>
+  <si>
+    <t>neuroblastoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005072</t>
+  </si>
+  <si>
+    <t>plasma cell neoplasm</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0004959</t>
+  </si>
+  <si>
+    <t>non-small cell lung carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term can be add as an ontology term</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPV can cause Back of the Throat, cervical (most) , Anus, vulva, penis, vagina cancer. Vaccine usually target the HPV virus.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fallopian tube cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0002158</t>
+  </si>
+  <si>
+    <t>small cell lung carcinoma</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +358,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,12 +384,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -246,6 +391,34 @@
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,14 +446,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -598,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F39B9E-8F82-5546-9B39-8E8CB52CC082}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -610,222 +792,428 @@
     <col min="2" max="2" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="19">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:3" ht="19">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19">
+      <c r="A15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19">
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19">
+      <c r="A18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="19">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19">
+      <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+    <row r="24" spans="1:2" ht="19">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="19">
+      <c r="A25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="19">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="19">
+      <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+    <row r="28" spans="1:2" ht="19">
+      <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+    <row r="29" spans="1:2" ht="19">
+      <c r="A29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19">
+      <c r="A30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="19">
+      <c r="A31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="19">
+      <c r="A32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19">
+      <c r="A33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19">
+      <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+    <row r="35" spans="1:2" ht="19">
+      <c r="A35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19">
+      <c r="A36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19">
+      <c r="A37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="19">
+      <c r="A38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="19">
+      <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="40" spans="1:2" ht="19">
+      <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>46</v>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19">
+      <c r="A41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19">
+      <c r="A42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19">
+      <c r="A43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19">
+      <c r="A44" s="3"/>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" ht="19">
+      <c r="A45" s="3"/>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" ht="19">
+      <c r="A46" s="3"/>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" ht="19">
+      <c r="A47" s="3"/>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" ht="19">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" ht="19">
+      <c r="A49" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19">
+      <c r="A50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{76B3671B-AE81-3B4D-B639-45BEA9A4A39E}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{6529AC54-0986-954A-ABFC-E7E0C48E0E8D}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{C0BD6991-4EF2-3940-8467-6895D5E56640}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{AB54BACF-4743-2440-B769-8969F799598F}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{311B2A2D-09F4-B34C-ABFA-A662256D2AEA}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{42218ABF-DF79-D14B-8E3E-3028200C9F1F}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{B9736674-A028-E64F-A68B-82BDA63D0196}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{9C33877D-B700-D648-856A-D92C0E2068F3}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{B049FB3B-7A6F-0448-A107-E0AB1C26A828}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{973A9DAA-F019-7846-805F-62448DBC6BB2}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{010106B8-E4FF-694E-9119-D5898A8C8410}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{A4266057-BBB8-884B-BF1A-5672017EEB7D}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{9C7A94ED-88FA-7240-AA31-3AF97B4D93BF}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{1C641ED4-88AC-0B43-A210-136324F48F68}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{439B6FD7-3AA5-EF4F-BB30-2C12AD840D1B}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{D04AF194-E214-3C4D-9CBE-F953545B7568}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{F39AD23A-4913-4941-9701-A41A489F7A08}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{8CF1754F-4A14-2147-82E6-D4C9BDFE02C1}"/>
-    <hyperlink ref="B19" r:id="rId19" display="http://purl.obolibrary.org/obo/MONDO_0009831" xr:uid="{1673021D-B51F-9D40-A9FA-80F9061F3504}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{C77CD132-89BD-0D40-A57F-FEA8E5696D29}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{F3D2B324-46CB-0640-A809-5B5FFDFB57E6}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{C6D653F5-699A-1A4B-9275-07680A0066BC}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{7A99A502-CE6C-7F4A-BCB8-BB78928D258D}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{76B3671B-AE81-3B4D-B639-45BEA9A4A39E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6529AC54-0986-954A-ABFC-E7E0C48E0E8D}"/>
+    <hyperlink ref="B23" r:id="rId3" xr:uid="{C0BD6991-4EF2-3940-8467-6895D5E56640}"/>
+    <hyperlink ref="B20" r:id="rId4" xr:uid="{AB54BACF-4743-2440-B769-8969F799598F}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{311B2A2D-09F4-B34C-ABFA-A662256D2AEA}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{42218ABF-DF79-D14B-8E3E-3028200C9F1F}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{B9736674-A028-E64F-A68B-82BDA63D0196}"/>
+    <hyperlink ref="B27" r:id="rId8" xr:uid="{9C33877D-B700-D648-856A-D92C0E2068F3}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{B049FB3B-7A6F-0448-A107-E0AB1C26A828}"/>
+    <hyperlink ref="B34" r:id="rId10" xr:uid="{973A9DAA-F019-7846-805F-62448DBC6BB2}"/>
+    <hyperlink ref="B39" r:id="rId11" xr:uid="{010106B8-E4FF-694E-9119-D5898A8C8410}"/>
+    <hyperlink ref="B40" r:id="rId12" xr:uid="{A4266057-BBB8-884B-BF1A-5672017EEB7D}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{1C641ED4-88AC-0B43-A210-136324F48F68}"/>
+    <hyperlink ref="B29" r:id="rId14" xr:uid="{439B6FD7-3AA5-EF4F-BB30-2C12AD840D1B}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{D04AF194-E214-3C4D-9CBE-F953545B7568}"/>
+    <hyperlink ref="B4" r:id="rId16" xr:uid="{F39AD23A-4913-4941-9701-A41A489F7A08}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{8CF1754F-4A14-2147-82E6-D4C9BDFE02C1}"/>
+    <hyperlink ref="B35" r:id="rId18" display="http://purl.obolibrary.org/obo/MONDO_0009831" xr:uid="{1673021D-B51F-9D40-A9FA-80F9061F3504}"/>
+    <hyperlink ref="B31" r:id="rId19" xr:uid="{C77CD132-89BD-0D40-A57F-FEA8E5696D29}"/>
+    <hyperlink ref="B37" r:id="rId20" xr:uid="{F3D2B324-46CB-0640-A809-5B5FFDFB57E6}"/>
+    <hyperlink ref="B9" r:id="rId21" xr:uid="{C6D653F5-699A-1A4B-9275-07680A0066BC}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{7A99A502-CE6C-7F4A-BCB8-BB78928D258D}"/>
+    <hyperlink ref="B2" r:id="rId23" xr:uid="{C882270D-7618-1A40-9CAB-93911EBEC10F}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{C94C1976-2AB0-774A-98BF-89CD420D4AA1}"/>
+    <hyperlink ref="B7" r:id="rId25" xr:uid="{BD513142-713C-9444-BBEE-DBE65ADF3F9C}"/>
+    <hyperlink ref="B10" r:id="rId26" xr:uid="{9C3F0B90-4011-D64C-8EE5-09F380FE3025}"/>
+    <hyperlink ref="B12" r:id="rId27" xr:uid="{FD18B493-A888-D74B-8129-7BAF6341C5ED}"/>
+    <hyperlink ref="B11" r:id="rId28" xr:uid="{BB0522EE-D669-C743-B02D-429E7F9A1DDE}"/>
+    <hyperlink ref="B14" r:id="rId29" xr:uid="{B1FF4B3F-5DD6-904B-8C2C-C9047117E6D5}"/>
+    <hyperlink ref="B15" r:id="rId30" xr:uid="{32F11EA7-6239-6548-93F0-13D7A7D7B5E6}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{12D46296-88D5-5F45-8649-5D3CAA495CCB}"/>
+    <hyperlink ref="B17" r:id="rId32" xr:uid="{BE668294-AA81-554C-A279-B47B72FF6BFD}"/>
+    <hyperlink ref="B18" r:id="rId33" xr:uid="{AAA170D7-381E-3640-8DEC-4678B9855AA0}"/>
+    <hyperlink ref="B42" r:id="rId34" xr:uid="{D70C253B-E05E-904E-B2E8-B43455467A4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update column has role has quality
</commit_message>
<xml_diff>
--- a/src/templates/cancer_vaccine_MONDO.xlsx
+++ b/src/templates/cancer_vaccine_MONDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB1E559-F253-5C42-80EF-0AF9D101A36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DAA2C9-C190-CA4D-BBF9-19F5AF463695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="680" windowWidth="28240" windowHeight="17040" xr2:uid="{922C2959-0093-1E49-9E88-C387A27C2EFD}"/>
   </bookViews>
@@ -782,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F39B9E-8F82-5546-9B39-8E8CB52CC082}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cancer_vaccine.csv has role and has quality column
</commit_message>
<xml_diff>
--- a/src/templates/cancer_vaccine_MONDO.xlsx
+++ b/src/templates/cancer_vaccine_MONDO.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CDD849-D025-334B-8092-8317E101C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DAA2C9-C190-CA4D-BBF9-19F5AF463695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="680" windowWidth="28240" windowHeight="17040" xr2:uid="{922C2959-0093-1E49-9E88-C387A27C2EFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>http://purl.obolibrary.org/obo/MONDO_0007254</t>
   </si>
@@ -106,16 +106,7 @@
     <t>renal cancer </t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/MONDO_0005089</t>
-  </si>
-  <si>
     <t>sarcoma</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/MONDO_0007576</t>
-  </si>
-  <si>
-    <t>esophageal cancer </t>
   </si>
   <si>
     <t>head and neck cancer</t>
@@ -175,10 +166,6 @@
     <t>http://purl.obolibrary.org/obo/MONDO_0005233</t>
   </si>
   <si>
-    <t>non-small cell lung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>prostate cancer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -199,7 +186,171 @@
     <t>lymphoma</t>
   </si>
   <si>
-    <t>disease</t>
+    <t>cancer name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MONDO or DOID link</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bile duct cancer</t>
+  </si>
+  <si>
+    <t>comments</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0003059</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>melanoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DOID_1909</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cholangiocarcinoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0019087</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>osteosarcoma</t>
+  </si>
+  <si>
+    <t>esophageal cancer</t>
+  </si>
+  <si>
+    <t>gastric adenocarcinoma</t>
+  </si>
+  <si>
+    <t>Ewing sarcoma</t>
+  </si>
+  <si>
+    <t>glioblastoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GVHD</t>
+  </si>
+  <si>
+    <t>head and neck squamous cell carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0007576</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005036</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0012817</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0018177</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0013730</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0009807</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0010150</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hematologic disorder</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005570</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPV associated cancer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lip and oral cavity carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0023644</t>
+  </si>
+  <si>
+    <t>oropharyngeal carcinoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0044926</t>
+  </si>
+  <si>
+    <t>rectal cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0006519</t>
+  </si>
+  <si>
+    <t>small intestine cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0000956</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005089</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mantle cell lymphoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0018876</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0008433</t>
+  </si>
+  <si>
+    <t>neuroblastoma</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0005072</t>
+  </si>
+  <si>
+    <t>plasma cell neoplasm</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0004959</t>
+  </si>
+  <si>
+    <t>non-small cell lung carcinoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term can be add as an ontology term</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPV can cause Back of the Throat, cervical (most) , Anus, vulva, penis, vagina cancer. Vaccine usually target the HPV virus.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fallopian tube cancer</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MONDO_0002158</t>
+  </si>
+  <si>
+    <t>small cell lung carcinoma</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +358,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,12 +384,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -246,6 +391,34 @@
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,14 +446,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -598,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F39B9E-8F82-5546-9B39-8E8CB52CC082}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -610,222 +792,428 @@
     <col min="2" max="2" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="19">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:3" ht="19">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19">
+      <c r="A15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19">
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19">
+      <c r="A18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="19">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19">
+      <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+    <row r="24" spans="1:2" ht="19">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="19">
+      <c r="A25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="19">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="19">
+      <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+    <row r="28" spans="1:2" ht="19">
+      <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+    <row r="29" spans="1:2" ht="19">
+      <c r="A29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19">
+      <c r="A30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="19">
+      <c r="A31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="19">
+      <c r="A32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19">
+      <c r="A33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19">
+      <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+    <row r="35" spans="1:2" ht="19">
+      <c r="A35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19">
+      <c r="A36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19">
+      <c r="A37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="19">
+      <c r="A38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="19">
+      <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="40" spans="1:2" ht="19">
+      <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>46</v>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19">
+      <c r="A41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19">
+      <c r="A42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19">
+      <c r="A43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19">
+      <c r="A44" s="3"/>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" ht="19">
+      <c r="A45" s="3"/>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" ht="19">
+      <c r="A46" s="3"/>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" ht="19">
+      <c r="A47" s="3"/>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" ht="19">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" ht="19">
+      <c r="A49" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19">
+      <c r="A50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{76B3671B-AE81-3B4D-B639-45BEA9A4A39E}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{6529AC54-0986-954A-ABFC-E7E0C48E0E8D}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{C0BD6991-4EF2-3940-8467-6895D5E56640}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{AB54BACF-4743-2440-B769-8969F799598F}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{311B2A2D-09F4-B34C-ABFA-A662256D2AEA}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{42218ABF-DF79-D14B-8E3E-3028200C9F1F}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{B9736674-A028-E64F-A68B-82BDA63D0196}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{9C33877D-B700-D648-856A-D92C0E2068F3}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{B049FB3B-7A6F-0448-A107-E0AB1C26A828}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{973A9DAA-F019-7846-805F-62448DBC6BB2}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{010106B8-E4FF-694E-9119-D5898A8C8410}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{A4266057-BBB8-884B-BF1A-5672017EEB7D}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{9C7A94ED-88FA-7240-AA31-3AF97B4D93BF}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{1C641ED4-88AC-0B43-A210-136324F48F68}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{439B6FD7-3AA5-EF4F-BB30-2C12AD840D1B}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{D04AF194-E214-3C4D-9CBE-F953545B7568}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{F39AD23A-4913-4941-9701-A41A489F7A08}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{8CF1754F-4A14-2147-82E6-D4C9BDFE02C1}"/>
-    <hyperlink ref="B19" r:id="rId19" display="http://purl.obolibrary.org/obo/MONDO_0009831" xr:uid="{1673021D-B51F-9D40-A9FA-80F9061F3504}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{C77CD132-89BD-0D40-A57F-FEA8E5696D29}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{F3D2B324-46CB-0640-A809-5B5FFDFB57E6}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{C6D653F5-699A-1A4B-9275-07680A0066BC}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{7A99A502-CE6C-7F4A-BCB8-BB78928D258D}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{76B3671B-AE81-3B4D-B639-45BEA9A4A39E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6529AC54-0986-954A-ABFC-E7E0C48E0E8D}"/>
+    <hyperlink ref="B23" r:id="rId3" xr:uid="{C0BD6991-4EF2-3940-8467-6895D5E56640}"/>
+    <hyperlink ref="B20" r:id="rId4" xr:uid="{AB54BACF-4743-2440-B769-8969F799598F}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{311B2A2D-09F4-B34C-ABFA-A662256D2AEA}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{42218ABF-DF79-D14B-8E3E-3028200C9F1F}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{B9736674-A028-E64F-A68B-82BDA63D0196}"/>
+    <hyperlink ref="B27" r:id="rId8" xr:uid="{9C33877D-B700-D648-856A-D92C0E2068F3}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{B049FB3B-7A6F-0448-A107-E0AB1C26A828}"/>
+    <hyperlink ref="B34" r:id="rId10" xr:uid="{973A9DAA-F019-7846-805F-62448DBC6BB2}"/>
+    <hyperlink ref="B39" r:id="rId11" xr:uid="{010106B8-E4FF-694E-9119-D5898A8C8410}"/>
+    <hyperlink ref="B40" r:id="rId12" xr:uid="{A4266057-BBB8-884B-BF1A-5672017EEB7D}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{1C641ED4-88AC-0B43-A210-136324F48F68}"/>
+    <hyperlink ref="B29" r:id="rId14" xr:uid="{439B6FD7-3AA5-EF4F-BB30-2C12AD840D1B}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{D04AF194-E214-3C4D-9CBE-F953545B7568}"/>
+    <hyperlink ref="B4" r:id="rId16" xr:uid="{F39AD23A-4913-4941-9701-A41A489F7A08}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{8CF1754F-4A14-2147-82E6-D4C9BDFE02C1}"/>
+    <hyperlink ref="B35" r:id="rId18" display="http://purl.obolibrary.org/obo/MONDO_0009831" xr:uid="{1673021D-B51F-9D40-A9FA-80F9061F3504}"/>
+    <hyperlink ref="B31" r:id="rId19" xr:uid="{C77CD132-89BD-0D40-A57F-FEA8E5696D29}"/>
+    <hyperlink ref="B37" r:id="rId20" xr:uid="{F3D2B324-46CB-0640-A809-5B5FFDFB57E6}"/>
+    <hyperlink ref="B9" r:id="rId21" xr:uid="{C6D653F5-699A-1A4B-9275-07680A0066BC}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{7A99A502-CE6C-7F4A-BCB8-BB78928D258D}"/>
+    <hyperlink ref="B2" r:id="rId23" xr:uid="{C882270D-7618-1A40-9CAB-93911EBEC10F}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{C94C1976-2AB0-774A-98BF-89CD420D4AA1}"/>
+    <hyperlink ref="B7" r:id="rId25" xr:uid="{BD513142-713C-9444-BBEE-DBE65ADF3F9C}"/>
+    <hyperlink ref="B10" r:id="rId26" xr:uid="{9C3F0B90-4011-D64C-8EE5-09F380FE3025}"/>
+    <hyperlink ref="B12" r:id="rId27" xr:uid="{FD18B493-A888-D74B-8129-7BAF6341C5ED}"/>
+    <hyperlink ref="B11" r:id="rId28" xr:uid="{BB0522EE-D669-C743-B02D-429E7F9A1DDE}"/>
+    <hyperlink ref="B14" r:id="rId29" xr:uid="{B1FF4B3F-5DD6-904B-8C2C-C9047117E6D5}"/>
+    <hyperlink ref="B15" r:id="rId30" xr:uid="{32F11EA7-6239-6548-93F0-13D7A7D7B5E6}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{12D46296-88D5-5F45-8649-5D3CAA495CCB}"/>
+    <hyperlink ref="B17" r:id="rId32" xr:uid="{BE668294-AA81-554C-A279-B47B72FF6BFD}"/>
+    <hyperlink ref="B18" r:id="rId33" xr:uid="{AAA170D7-381E-3640-8DEC-4678B9855AA0}"/>
+    <hyperlink ref="B42" r:id="rId34" xr:uid="{D70C253B-E05E-904E-B2E8-B43455467A4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>